<commit_message>
remove left over ontology refs
</commit_message>
<xml_diff>
--- a/templates/community/TRR341_Phenotyping/Assay_Phenotyping_protocol_TRR341_MIAPPE.xlsx
+++ b/templates/community/TRR341_Phenotyping/Assay_Phenotyping_protocol_TRR341_MIAPPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie Jacquemin\Documents\GitHub\Swate-templates_myfork\templates\community\TRR341_Phenotyping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/community/TRR341_Phenotyping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1316150E-27E9-4933-B1D6-E012BB49EADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BADFE56-8D52-A04F-9EA2-26BEB73514A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="3090" windowWidth="13260" windowHeight="11145" activeTab="1" xr2:uid="{C1162DCB-69E8-42CC-B926-8705FE9A7104}"/>
+    <workbookView xWindow="-24360" yWindow="-21100" windowWidth="35880" windowHeight="18680" xr2:uid="{C1162DCB-69E8-42CC-B926-8705FE9A7104}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotyping_protocol" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="61">
   <si>
     <t/>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>Phenotyping</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/PO_0009005</t>
-  </si>
-  <si>
-    <t>PO</t>
   </si>
   <si>
     <t>Parameter [Trait Definition File]</t>
@@ -798,29 +792,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A36DA2E-E291-4ECD-B08C-389CC67174F7}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="38.28515625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="38.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -834,25 +828,25 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
         <v>4</v>
@@ -861,22 +855,18 @@
         <v>3</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
@@ -928,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -962,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -996,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1030,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1064,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1098,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1132,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1166,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1212,216 +1202,216 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639CE30E-7ABF-41AC-97E0-69E353E9D677}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="3" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="11" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="B27" s="9"/>
     </row>

</xml_diff>

<commit_message>
add ontology reference to tag in TRR MIAPPE templates
</commit_message>
<xml_diff>
--- a/templates/community/TRR341_Phenotyping/Assay_Phenotyping_protocol_TRR341_MIAPPE.xlsx
+++ b/templates/community/TRR341_Phenotyping/Assay_Phenotyping_protocol_TRR341_MIAPPE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\community\TRR341_Phenotyping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC5B10F-0BE7-46AE-9930-ED7407E010F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7E123C-0E4E-4E1B-ADAC-1E138543FCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C1162DCB-69E8-42CC-B926-8705FE9A7104}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="64">
   <si>
     <t/>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>DPBO:1000224</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C52095</t>
+  </si>
+  <si>
+    <t>NCIT</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1215,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1316,7 +1322,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1325,6 +1331,9 @@
       </c>
       <c r="C13" s="12" t="s">
         <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
       </c>
       <c r="E13" t="s">
         <v>60</v>
@@ -1335,6 +1344,9 @@
         <v>29</v>
       </c>
       <c r="B14" s="3"/>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update tags in TRR MIAPPE templates
</commit_message>
<xml_diff>
--- a/templates/community/TRR341_Phenotyping/Assay_Phenotyping_protocol_TRR341_MIAPPE.xlsx
+++ b/templates/community/TRR341_Phenotyping/Assay_Phenotyping_protocol_TRR341_MIAPPE.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\community\TRR341_Phenotyping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7E123C-0E4E-4E1B-ADAC-1E138543FCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BAE4F0-2614-4064-908B-D567EFE1C7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C1162DCB-69E8-42CC-B926-8705FE9A7104}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C1162DCB-69E8-42CC-B926-8705FE9A7104}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotyping_protocol" sheetId="3" r:id="rId1"/>
     <sheet name="isa_template" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -184,9 +184,6 @@
     <t>annotationTableSlimyQuail8</t>
   </si>
   <si>
-    <t xml:space="preserve"> metadata </t>
-  </si>
-  <si>
     <t>assay</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>NCIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metadata </t>
   </si>
 </sst>
 </file>
@@ -1215,13 +1215,14 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1307,19 +1308,19 @@
         <v>27</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
         <v>49</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1327,16 +1328,16 @@
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="E13" t="s">
         <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1345,7 +1346,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" s="12"/>
     </row>
@@ -1360,7 +1361,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1368,7 +1369,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1382,7 +1383,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1408,7 +1409,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1422,7 +1423,7 @@
         <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>